<commit_message>
[main] Updated formatting (2021-09-29-1220)
</commit_message>
<xml_diff>
--- a/src/un_sdg/data/un_sdg.xlsx
+++ b/src/un_sdg/data/un_sdg.xlsx
@@ -2488,13 +2488,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>